<commit_message>
Cambios en excel de productos
</commit_message>
<xml_diff>
--- a/public/assets/files/PlantillaClientes.xlsx
+++ b/public/assets/files/PlantillaClientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissa/Dropbox/phormo/etax/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7EC47D4-CFF3-4B38-81CF-04CD563DBD6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98946822-B3DA-764B-ADA1-3D4CC027B589}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,811 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>eTax</author>
+    <author>Usuario de Microsoft Office</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{67B67D71-C017-D54B-B812-D9D1E1A544AA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Código de cliente:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">El código de cliente es un código definido por usted que se utiliza para ordenar  sus clientes en eTax.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>Digite el código previamente creado en eTax para clientes existentes, o bien, defina un código nuevo para clientes nuevos.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{0F97FF03-7BDD-DB4C-A6E6-8D9FE7E44477}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Código de identificación:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 - Cédula física
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 - Cédula jurídica
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 - DIMEX
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 - NITE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 - Extranjero
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 - Otro</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{173BBB13-FA4B-194B-ABB9-6581029A45CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sobre el número de identificación:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Escriba el número sin guiones. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>En el caso de cédulas físicas, el número debe contener 9 dígitos. Si el número de cédula es más corto, complete con ceros.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="1" shapeId="0" xr:uid="{27BED091-8A71-DA46-A3B4-5E74EEAE8896}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sobre el correo electrónico:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>En caso de utilizar eTax como sistema de facturación electrónica, este será el correo al que se le enviará la factura electrónica y demás documentación.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{11909824-D6D8-334F-8EDE-290E5D78864B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>País:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Utilice como guía el documento adjunto.
+La sigla debe tener dos letras.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{A7E26DD4-BD0D-1140-9801-66B19D7B248B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Provincias de Costa Rica:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 - San José
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 - Alajuela
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 - Cartago 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 - Heredia
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 - </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guanacaste</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">6 - Puntarenas
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">7 - Limón
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>En caso de que el país NO sea Costa Rica, escriba el nombre correspondiente a la provincia.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{BD03C317-448D-CE4B-8399-DAC7A3D29874}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cantón:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Utilize como guía el documento adjunto para identificar el código que corresponde. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El código es un número de 3 dígitos donde el primer número corresponde al número de provincia y los siguientes dos al número de cantón dentro de la provincia.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>En caso de que el país NO sea Costa Rica, escriba el nombre correspondiente al cantón.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{E81F30FA-8A15-754F-BB5B-5547CE184240}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Distrito:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Utilize como guía el documento adjunto para identificar el código que corresponde. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El código es un número de 5 dígitos donde el primer número corresponde al número de provincia, los siguientes dos al número de cantón y los últimos dos al número de distrito.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>En caso de que el país NO sea Costa Rica, escriba el nombre correspondiente al distrito.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="1" shapeId="0" xr:uid="{3277290E-2966-6648-BEAA-AF1E2E1303DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Barrio:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Utilice como guía el documento adjunto para identificar los nombres oficiales de barrios. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">En caso de que el país NO sea Costa Rica, escriba el nombre correspondiente </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>al barrio.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="1" shapeId="0" xr:uid="{029FCB90-D2D3-DB47-9360-A7AA53EDA67D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Sobre el código de área:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Para Costa Rica, digitar 506</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{0A707099-F723-AD4F-98E6-BA36704E79C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sobre la copia del correo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Si no desea enviar copias, deje en blanco.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Codigo</t>
   </si>
@@ -85,18 +888,12 @@
     <t>CODEJ</t>
   </si>
   <si>
-    <t>Cliente Ejemplo</t>
-  </si>
-  <si>
     <t>Apelllido1</t>
   </si>
   <si>
     <t>Apellido2</t>
   </si>
   <si>
-    <t>1-XXXX-XXXX</t>
-  </si>
-  <si>
     <t>nombre@correo.com</t>
   </si>
   <si>
@@ -104,13 +901,98 @@
   </si>
   <si>
     <t>1234-1234</t>
+  </si>
+  <si>
+    <t>Indique el código de cliente utilizado en eTax.</t>
+  </si>
+  <si>
+    <t>Elija el código equivalente al tipo de identificación del cliente.</t>
+  </si>
+  <si>
+    <t>Indíque el número de identificación del cliente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bienvenido al sistema de importación de clientes vía excel de eTax. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Complete los datos de sus clientes en las celdas corresopndientes (a partir de la fila 4, inclusive). Cada cliente se detalla en su propia fila.
+Pase su cursor por las celdas de la segunda fila marcadas con un triángulo en la esquina superior derecha para ver más detalles sobre la información que debe digitar.
+No modifique los textos de la tercera fila. Estos son necesarios para la correcta lectura del documento.</t>
+    </r>
+  </si>
+  <si>
+    <t>Indique en siglas el país del cliente</t>
+  </si>
+  <si>
+    <t>XXXXXXXXX</t>
+  </si>
+  <si>
+    <t>Indique el número que corresponde a la provincia del cliente.</t>
+  </si>
+  <si>
+    <t>Indique el nombre del cliente</t>
+  </si>
+  <si>
+    <t>Indique el primer apellido del cliente</t>
+  </si>
+  <si>
+    <t>Indique el segundo apellido del cliente</t>
+  </si>
+  <si>
+    <t>Indique el correo electrónico del cliente.</t>
+  </si>
+  <si>
+    <t>Elija el número que corresponde al cantón del cliente.</t>
+  </si>
+  <si>
+    <t>Elija el número que corresponde al distrito del cliente.</t>
+  </si>
+  <si>
+    <t>Indíque el barrio del cliente.</t>
+  </si>
+  <si>
+    <t>Indique la dirección del cliente</t>
+  </si>
+  <si>
+    <t>Indique el código de área del teléfono del cliente de acuerdo al país.</t>
+  </si>
+  <si>
+    <t>Indique el número de teléfono</t>
+  </si>
+  <si>
+    <t>Indique la dirección de correo electrónico a la que se le enviará una copia de la factura electrónica.</t>
+  </si>
+  <si>
+    <t>Elija la opción que indica si el cliente regularmente está exento (SÍ) o no (NO)</t>
+  </si>
+  <si>
+    <t>Indique si el cliente es emisor (E), receptor (R), o emisor y receptor de facturación electrónia (ER)</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -120,6 +1002,48 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,12 +1067,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -165,8 +1108,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R2">
-  <autoFilter ref="A1:R2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:R4">
+  <autoFilter ref="A3:R4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Codigo"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nombre"/>
@@ -174,7 +1117,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SegundoApellido"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TipoPersona"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Identificacion"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Correo" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Correo"/>
     <tableColumn id="19" xr3:uid="{D31E5BE9-9174-423A-ACFA-BD29570B1F95}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Provincia"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Canton"/>
@@ -183,7 +1126,7 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Direccion"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="AreaTel"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Telefono"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CorreosCopia" dataCellStyle="Hyperlink"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CorreosCopia"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Exento"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="EmisorReceptor"/>
   </tableColumns>
@@ -192,7 +1135,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -487,135 +1430,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="18" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+    </row>
+    <row r="2" spans="1:23" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M3" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O3" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q3" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J4">
+        <v>101</v>
+      </c>
+      <c r="K4">
+        <v>10101</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>101</v>
-      </c>
-      <c r="K2">
-        <v>10101</v>
-      </c>
-      <c r="L2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
+      <c r="P4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:W1"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{FB5AAD66-7B56-EC41-89B1-925E7155AB49}">
+      <formula1>"1, 2, 3, 4, 5, 6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R4" xr:uid="{FD64E9DF-C202-6D40-8A35-F9E0D6012FAE}">
+      <formula1>"E,R,ER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4" xr:uid="{3F792A50-2C73-3045-9F03-4CB2152D0231}">
+      <formula1>"SÍ,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{29DD8F2F-81ED-46C6-998A-A4AB7A019606}"/>
-    <hyperlink ref="P2" r:id="rId2" xr:uid="{FFE41E9D-3233-495D-BE64-74207D3A2BEF}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{29DD8F2F-81ED-46C6-998A-A4AB7A019606}"/>
+    <hyperlink ref="P4" r:id="rId2" xr:uid="{FFE41E9D-3233-495D-BE64-74207D3A2BEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>